<commit_message>
DisAssembly WO changes. Removed .secrete file from project
</commit_message>
<xml_diff>
--- a/templates/Disassembly Work Order.xlsx
+++ b/templates/Disassembly Work Order.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B553017E-60F9-4CEA-AA0F-6168F7649000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74524D20-2F1E-4401-9D37-F3E51C1C878A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="19200" windowHeight="8520" activeTab="1" xr2:uid="{410C97DE-4098-431C-AD23-B1A3C3378843}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{410C97DE-4098-431C-AD23-B1A3C3378843}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Disassembly WO" sheetId="1" r:id="rId1"/>
-    <sheet name="Consumable Components" sheetId="2" r:id="rId2"/>
+    <sheet name="Derived Components" sheetId="3" r:id="rId2"/>
+    <sheet name="Consumable Components" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">Work Order number </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
   <si>
     <t>Disassembly item name</t>
   </si>
@@ -55,19 +53,100 @@
     <t>Component Item</t>
   </si>
   <si>
-    <t>Qty Per</t>
-  </si>
-  <si>
-    <t>Work Order Number</t>
-  </si>
-  <si>
     <t>MS-Disassembly (NO Track)</t>
   </si>
   <si>
     <t>MS-serial and lot tracked (mfg lot and serial)</t>
   </si>
   <si>
-    <t>Provar-61</t>
+    <t>Derived Component Item</t>
+  </si>
+  <si>
+    <t>Expected Qty</t>
+  </si>
+  <si>
+    <t>Actual Yield Qty</t>
+  </si>
+  <si>
+    <t>Cost Allocation Pct</t>
+  </si>
+  <si>
+    <t>Disassy Good Loc ID</t>
+  </si>
+  <si>
+    <t>Disassy Good Loc No</t>
+  </si>
+  <si>
+    <t>Responsible User</t>
+  </si>
+  <si>
+    <t>Add derived Component?</t>
+  </si>
+  <si>
+    <t>Lot Number</t>
+  </si>
+  <si>
+    <t>Lot Exp Date</t>
+  </si>
+  <si>
+    <t>Ms-child2 (Lot track)</t>
+  </si>
+  <si>
+    <t>Ms-child3 (Serial item)</t>
+  </si>
+  <si>
+    <t>Ms-child4 (Serial and item)</t>
+  </si>
+  <si>
+    <t>DisLot-1</t>
+  </si>
+  <si>
+    <t>Enter Qty Per Flag</t>
+  </si>
+  <si>
+    <t>Enter Component Qty Flag</t>
+  </si>
+  <si>
+    <t>Fixed Component Qty Flag</t>
+  </si>
+  <si>
+    <t>Component Qty</t>
+  </si>
+  <si>
+    <t>Scrap Factor</t>
+  </si>
+  <si>
+    <t>Setup Qty</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Pro-child4 (NO Track)</t>
+  </si>
+  <si>
+    <t>Component Per</t>
+  </si>
+  <si>
+    <t>Pro-child5 (NO Track)</t>
+  </si>
+  <si>
+    <t>Fixed Qty</t>
+  </si>
+  <si>
+    <t>Add consumable components?</t>
+  </si>
+  <si>
+    <t>Mayur Suryawanshi</t>
+  </si>
+  <si>
+    <t>Pro-Disassembley (Lot and serial track)</t>
+  </si>
+  <si>
+    <t>Pro-Disassembley Serial (Serial track)</t>
+  </si>
+  <si>
+    <t>Pro-Disassembley Lot (Lot track)</t>
   </si>
 </sst>
 </file>
@@ -103,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,21 +499,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9D0080-B4D2-4351-9E4B-3E7D4A08CBFC}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,32 +525,92 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -478,47 +619,508 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A55D77-3A07-4BB8-BFD8-EAD99132AF4E}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72AE76E0-FB9A-4E01-B002-1F029404FF4C}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1">
+        <v>44966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A55D77-3A07-4BB8-BFD8-EAD99132AF4E}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="G3">
+        <v>1E-3</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1E-3</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>1E-3</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>1E-3</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.3</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Complete flow for Rework WO Added Complete flow for Refurb WO Added Complete flow for Consigned WO Added Complete flow for Labor WO
</commit_message>
<xml_diff>
--- a/templates/Disassembly Work Order.xlsx
+++ b/templates/Disassembly Work Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74524D20-2F1E-4401-9D37-F3E51C1C878A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C54A3DC-AE42-4C59-8DC5-1F53F2EDD923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{410C97DE-4098-431C-AD23-B1A3C3378843}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{410C97DE-4098-431C-AD23-B1A3C3378843}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Disassembly WO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
   <si>
     <t>Disassembly item name</t>
   </si>
@@ -499,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9D0080-B4D2-4351-9E4B-3E7D4A08CBFC}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,20 +599,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,7 +609,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A55D77-3A07-4BB8-BFD8-EAD99132AF4E}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>